<commit_message>
correccion de bugs y agrego de seleccion de carpeta para la generacion de reportes
</commit_message>
<xml_diff>
--- a/src/informesGenerados/ResumenMINCOM.xlsx
+++ b/src/informesGenerados/ResumenMINCOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Tipo</t>
   </si>
@@ -98,235 +98,265 @@
     <t>Pérdidas (MN)</t>
   </si>
   <si>
+    <t>2019-02-01</t>
+  </si>
+  <si>
+    <t>DTMZ</t>
+  </si>
+  <si>
+    <t>Sustracción del transformador de la fuente de alimentación a una EP. Mercado Ideal -Cayo Ramona</t>
+  </si>
+  <si>
+    <t>Avería PExt</t>
+  </si>
+  <si>
+    <t>DTSS</t>
+  </si>
+  <si>
+    <t>Partido poste de madera de 7.5 mts, por accidente de tránsito. Calles Luz y Caballero No. 62,  entre Frank País y Tirso Marín</t>
+  </si>
+  <si>
+    <t>2019-02-05</t>
+  </si>
+  <si>
+    <t>DTCM</t>
+  </si>
+  <si>
+    <t>Partido cable multipar de 600 pares por accidente de tránsito. Calle Maceo</t>
+  </si>
+  <si>
+    <t>DTGR</t>
+  </si>
+  <si>
+    <t>Partida FO, por accidente de tránsito. Localidad La Norma</t>
+  </si>
+  <si>
+    <t>2019-02-06</t>
+  </si>
+  <si>
+    <t>Quemadas varias regletas y jumpers de un gabinete, por toque eléctrico. Circunvalación Norte</t>
+  </si>
+  <si>
+    <t>Robo</t>
+  </si>
+  <si>
+    <t>DTLT</t>
+  </si>
+  <si>
+    <t>Sustracción de moto Jawa 350.  Biplanta D. Apto 4. Localidad Aguilera</t>
+  </si>
+  <si>
+    <t>Acc. Tránsito</t>
+  </si>
+  <si>
+    <t>2019-02-07</t>
+  </si>
+  <si>
+    <t>DCNI</t>
+  </si>
+  <si>
+    <t>Accidente de tránsito sin lesionados, no imputable a ETECSA. Calle Perla y San Ignacio</t>
+  </si>
+  <si>
+    <t>2019-02-08</t>
+  </si>
+  <si>
+    <t>DTMY</t>
+  </si>
+  <si>
+    <t>Partido poste de madera de 7.5 mts, por accidente de tránsito. Central Héctor Molina</t>
+  </si>
+  <si>
+    <t>2019-02-09</t>
+  </si>
+  <si>
+    <t>DTSC</t>
+  </si>
+  <si>
+    <t>Sustraídas 4 tarjetas magnéticas a una ejecutiva del CAT por otra trabajadora. Calle Aguilera No. 401,  entre Calvario y Carnicería</t>
+  </si>
+  <si>
     <t>Delito vs PExt</t>
   </si>
   <si>
-    <t>2021-01-06</t>
-  </si>
-  <si>
-    <t>DTCM</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte de FO. Ave.Finlay. Nuevitas</t>
-  </si>
-  <si>
-    <t>2021-01-07</t>
-  </si>
-  <si>
-    <t>DTMZ</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte de FO. Batey de Junco hacia La Carlota</t>
-  </si>
-  <si>
-    <t>Avería PExt</t>
-  </si>
-  <si>
-    <t>DTGT</t>
-  </si>
-  <si>
-    <t>Parido poste de hormigón de 7.5 mts, por accidente de tránsito. Carretera Principal Argeo Martínez</t>
-  </si>
-  <si>
-    <t>2021-01-08</t>
+    <t>2019-02-12</t>
+  </si>
+  <si>
+    <t>DTIJ</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Calle 41 No. 4614,  entre 46 y 52</t>
+  </si>
+  <si>
+    <t>Fracturados los microteléfonos a 2 EP. Calle 13. Puerto de Manatí</t>
+  </si>
+  <si>
+    <t>2019-02-14</t>
+  </si>
+  <si>
+    <t>Partido poste de hormigón de 9.00 mts,  por accidente de tránsito. Calle 26, entre Vicente Quesada y José A. Echevarría</t>
+  </si>
+  <si>
+    <t>2019-02-15</t>
+  </si>
+  <si>
+    <t>DTCF</t>
+  </si>
+  <si>
+    <t>Fracturado microteléfono a una EP. Calle 63, entre 54 y 56</t>
+  </si>
+  <si>
+    <t>Partidos 3 postes de hormigón de 9.00 mts, por accidente del tránsito. Cuatro camino entrada de Calimete</t>
+  </si>
+  <si>
+    <t>2019-02-16</t>
+  </si>
+  <si>
+    <t>Sustracción de herramientas del interior de un vehículo. Hotel Guacanayabo</t>
+  </si>
+  <si>
+    <t>Incendio Ext.</t>
+  </si>
+  <si>
+    <t>DTVC</t>
+  </si>
+  <si>
+    <t>Quemados cables multipares de 400 y 20 pares por toque eléctrico. Calle Esquerra, entre Independencia y Martí</t>
+  </si>
+  <si>
+    <t>2019-02-17</t>
+  </si>
+  <si>
+    <t>Partida la FO aérea, por caída de ábol. Cuatro Esquinas de Santa Lucía</t>
+  </si>
+  <si>
+    <t>2019-02-18</t>
+  </si>
+  <si>
+    <t>Partido cable de 200 pares y ramal de 30 pares, por combinada cañera. Localidad Haití</t>
+  </si>
+  <si>
+    <t>Fracturado microteléfono a una EP. Reparto Siboney. Guamo</t>
+  </si>
+  <si>
+    <t>2019-02-19</t>
+  </si>
+  <si>
+    <t>DESP</t>
+  </si>
+  <si>
+    <t>Accidente de tránsito sin lesionados, no imputable a ETECSA. Calle 27 entre 72 y 74</t>
+  </si>
+  <si>
+    <t>Sustracción de cápsula receptora con su tapa a una E.P. Avenida 60,  entre 73 y 75</t>
+  </si>
+  <si>
+    <t>DTHO</t>
+  </si>
+  <si>
+    <t>Sustracción de microteléfono a una EP. Calle Juan Sierra, entre Antonio Maceo y Carlos M. de Céspedes.</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Calle Paraiso, entre Cisnero y Lora</t>
+  </si>
+  <si>
+    <t>2019-02-20</t>
+  </si>
+  <si>
+    <t>Partido microteléfono a una EP. Localidad Rural Playa Florida</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de cable tensor. Localidad Guaranal</t>
+  </si>
+  <si>
+    <t>DTES</t>
+  </si>
+  <si>
+    <t>Partida FO, por accidente de tránsito. Callejón El sapo</t>
+  </si>
+  <si>
+    <t>2019-02-21</t>
+  </si>
+  <si>
+    <t>Afectación a la planta exterior por corte y sustracción de cable tensor. Carretera San Germán a 1 Km del vertedero</t>
+  </si>
+  <si>
+    <t>2019-02-22</t>
+  </si>
+  <si>
+    <t>DTSR</t>
+  </si>
+  <si>
+    <t>Afectación a cable de 200 pares por trabajos de la Empresa Eléctrica. Calle Reforma entre  Calzada de Luyano</t>
+  </si>
+  <si>
+    <t>2019-02-23</t>
+  </si>
+  <si>
+    <t>Accidente de tránsito sin lesionados, no imputable a ETECSA. Avenida de las Americas. Inmediaciones del Teatro Teatro Heredia. Avenida las Américas</t>
+  </si>
+  <si>
+    <t>2019-02-24</t>
+  </si>
+  <si>
+    <t>Sustracción del microteléfono a una EP. Calle Leal y Primera</t>
+  </si>
+  <si>
+    <t>2019-02-25</t>
+  </si>
+  <si>
+    <t>DTAR</t>
+  </si>
+  <si>
+    <t>Partido poste de madera de 9.00 mts, por accidente de tránsito. Calle 61, entre 72 y 80</t>
   </si>
   <si>
     <t>DTCA</t>
   </si>
   <si>
-    <t>Partido Microteléfono a una EP. Tienda de víveres del Batey Eduviges Sanguily</t>
-  </si>
-  <si>
-    <t>Incendio Ext.</t>
-  </si>
-  <si>
-    <t>DTPR</t>
-  </si>
-  <si>
-    <t>Moto incendiada por corto circuito, durante su reparación. Avenida Borrego, entre Calle R Formell y Calle B</t>
+    <t>Intento de Robo Minipunto Máximo Gómez. Calle Máximo Gómez, entre 1 y 2</t>
+  </si>
+  <si>
+    <t>Partido poste de hormigón de 7.00 mts, por accidente de tránsito. Carretera Boca de Camarioca- La Conchita</t>
+  </si>
+  <si>
+    <t>Vandalizada una EP. Unidad Militar 2100. Carretera Monumental Km 11 1/2</t>
+  </si>
+  <si>
+    <t>2019-02-26</t>
+  </si>
+  <si>
+    <t>DCEC</t>
+  </si>
+  <si>
+    <t>Accidente de tránsito no imputable a ETECSA, sin lesionados. 5ta Avenida y 112.</t>
+  </si>
+  <si>
+    <t>2019-02-27</t>
   </si>
   <si>
     <t>DTOE</t>
   </si>
   <si>
-    <t>Sustracción del microteléfono a una EP. Calle 300</t>
-  </si>
-  <si>
-    <t>Acc. Tránsito</t>
-  </si>
-  <si>
-    <t>CTC</t>
-  </si>
-  <si>
-    <t>Accidente de tránsito no imputable a ETECSA, sin lesionados. Calle Infanta y Salvador Allende</t>
-  </si>
-  <si>
-    <t>Robo</t>
-  </si>
-  <si>
-    <t>2021-01-11</t>
-  </si>
-  <si>
-    <t>Intento de robo Minipunto. Rpto. Fructuoso Rodríguez</t>
-  </si>
-  <si>
-    <t>Desprendida de la pared y abondonada en el suelo una EP. Rpto. Biplanta- Avenida Salva, entre calle 17 y calle 17 B</t>
-  </si>
-  <si>
-    <t>2021-01-12</t>
-  </si>
-  <si>
-    <t>DTCF</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte y sustracción de cable telefónico. UBPC Turquino</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte de cable telefónico de 200 pares. Km 3/2. Punta Brava</t>
-  </si>
-  <si>
-    <t>DTSR</t>
-  </si>
-  <si>
-    <t>Partido cable de 50 pares, por accidente del tránsito. Calle Rafael de Cardenas, entre 3ra y 4ta</t>
-  </si>
-  <si>
-    <t>DTES</t>
-  </si>
-  <si>
-    <t>Sustracción de lámparas LED. Avenidad Rotaria,  entre Ciruela y Enlace</t>
-  </si>
-  <si>
-    <t>2021-01-13</t>
-  </si>
-  <si>
-    <t>Partido un poste de madera de 7.5 mts y dos cables telefónicos, por accidente de tránsito. Calle Augusto Arango</t>
-  </si>
-  <si>
-    <t>DVLS</t>
-  </si>
-  <si>
-    <t>Sustracción de un televisor. Avenida Los Pinos y 3ra. Sevillano</t>
-  </si>
-  <si>
-    <t>2021-01-14</t>
-  </si>
-  <si>
-    <t>DECA</t>
-  </si>
-  <si>
-    <t>Accidente del tránsito imputable a ETECSA, sin lesionados. Entrada Tunel de la Habana</t>
-  </si>
-  <si>
-    <t>2021-01-15</t>
-  </si>
-  <si>
-    <t>Golpeado tubo soterrado, por labores de constructivas de la empresa ARCOS. Carretera Las Américas</t>
-  </si>
-  <si>
-    <t>2021-01-18</t>
-  </si>
-  <si>
-    <t>DTSC</t>
-  </si>
-  <si>
-    <t>Accidente de tránsito sin lesionados, imputable a ETECSA. Barrio Comunidad Militar</t>
-  </si>
-  <si>
-    <t>2021-01-20</t>
-  </si>
-  <si>
-    <t>DTGR</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte y sustracción de tensor. Km 2. Carretera Bayamo</t>
-  </si>
-  <si>
-    <t>Intento de robo en minipunto. Calle 30, entre Carrillo y Saez</t>
-  </si>
-  <si>
-    <t>DTVC</t>
-  </si>
-  <si>
-    <t>Partido poste madera de 9.00 mts y cable de FO, por accidente de tránsito. Localidad Quemado de Güines</t>
-  </si>
-  <si>
-    <t>2021-01-21</t>
-  </si>
-  <si>
-    <t>Partido poste de madera de 9.00 mts y FO. Entronque del batey 6 de Agosto</t>
-  </si>
-  <si>
-    <t>2021-01-22</t>
-  </si>
-  <si>
-    <t>Accidente de tránsito sin lesionados, imputable a ETECSA. Calle Fabrica. No. 54,  entre Aspuru y Línea del FC</t>
-  </si>
-  <si>
-    <t>2021-01-23</t>
-  </si>
-  <si>
-    <t>Partido cable multipar de 100 pares, por accidente de tránsito. Carretera a Esmeralda</t>
-  </si>
-  <si>
-    <t>DTLT</t>
-  </si>
-  <si>
-    <t>Interno con un machete causa daño multiples a una EP. Carretera Manatí.  Centro Penitenciario La Estrella</t>
-  </si>
-  <si>
-    <t>DTSS</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Calle José Martí, entre A y B</t>
-  </si>
-  <si>
-    <t>2021-01-25</t>
-  </si>
-  <si>
-    <t>DTMY</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte de cable coaxial. Carretera a Cayajabos, entre Repetidor 3 y Repetidor 4</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte y sustracción de tensor. Carretera a Sábalo</t>
-  </si>
-  <si>
-    <t>2021-01-27</t>
-  </si>
-  <si>
-    <t>Partidos 2 postes de madera de 7.00 mts, por accidente de tránsito. Calle Retiro, entre Méndez Capote y Acueducto</t>
-  </si>
-  <si>
-    <t>2021-01-28</t>
+    <t>Vandalizada una EP. Calle 51, entre 158 y 160</t>
+  </si>
+  <si>
+    <t>2019-02-28</t>
+  </si>
+  <si>
+    <t>Partido poste de hormigón de 9.00 mts, por accidente de tránsito. calle Camilo Cienfuego. Esq. Restaurante Las Palmeras</t>
   </si>
   <si>
     <t>DTNO</t>
   </si>
   <si>
-    <t>Accidente de transito con lesionados, no imputable a ETECSA. Entre Calle Zapata y Paseo</t>
-  </si>
-  <si>
-    <t>2021-01-29</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte y sustracción de cable telefónico. Camino a la localidad La Pimienta</t>
-  </si>
-  <si>
-    <t>Afectación a la planta exterior por corte y sustracción de bajante telefónico. Carretera de Baconao KM 1 1/2</t>
+    <t>Accidente de transito sin lesionados, imputable a ETECSA. Calzada de 10 de Octubre  y Santa Catalina</t>
   </si>
   <si>
     <t>DVLH</t>
   </si>
   <si>
-    <t>Accidente de tránsito con lesionados,  no imputable. Entre Calle Monte y Rastro</t>
-  </si>
-  <si>
-    <t>2021-01-31</t>
-  </si>
-  <si>
-    <t>Partido poste de hormigón de 9.00 mts y cable de 30 pares por accidente de tránsito. Ave 64 y Esquina 49</t>
+    <t>Sustracción de Laptop del interior de un vehículo. Calle Galiano y Concordia</t>
   </si>
 </sst>
 </file>
@@ -623,10 +653,10 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="????? Light"/>
-        <a:font script="Hang" typeface="?? ??"/>
-        <a:font script="Hans" typeface="?? Light"/>
-        <a:font script="Hant" typeface="????"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -675,10 +705,10 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="?????"/>
-        <a:font script="Hang" typeface="?? ??"/>
-        <a:font script="Hans" typeface="??"/>
-        <a:font script="Hant" typeface="????"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -911,13 +941,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C3" s="6">
-        <v>0</v>
+        <v>7759.54</v>
       </c>
       <c r="D3" s="7">
-        <v>7108.6</v>
+        <v>412.74</v>
       </c>
     </row>
     <row r="4">
@@ -925,13 +955,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="6">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6">
-        <v>0</v>
+        <v>580.14</v>
       </c>
       <c r="D4" s="7">
-        <v>774.58</v>
+        <v>211.18</v>
       </c>
     </row>
     <row r="5">
@@ -939,13 +969,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6">
-        <v>0</v>
+        <v>2004.31</v>
       </c>
       <c r="D5" s="7">
-        <v>2340</v>
+        <v>1892.52</v>
       </c>
     </row>
     <row r="6">
@@ -1020,13 +1050,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="6">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C11" s="6">
-        <v>0</v>
+        <v>1365.25</v>
       </c>
       <c r="D11" s="7">
-        <v>153</v>
+        <v>2797.2900000000004</v>
       </c>
     </row>
     <row r="12">
@@ -1079,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="6">
-        <v>0</v>
+        <v>464.82</v>
       </c>
       <c r="D15" s="7">
-        <v>0</v>
+        <v>49.14</v>
       </c>
     </row>
     <row r="16">
@@ -1149,8 +1179,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A2:D2"/>
     <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="100" paperSize="9" fitToWidth="0" fitToHeight="0" horizontalDpi="0" verticalDpi="0" copies="1"/>
@@ -1160,7 +1190,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
   <sheetPr/>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -1195,136 +1225,136 @@
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>30</v>
-      </c>
       <c r="E2" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F2" s="7">
-        <v>10.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>33</v>
-      </c>
       <c r="E3" s="6">
-        <v>0</v>
+        <v>133.09</v>
       </c>
       <c r="F3" s="7">
-        <v>1868</v>
+        <v>300.66</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="6">
         <v>0</v>
       </c>
       <c r="F4" s="7">
-        <v>0</v>
+        <v>644.7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" s="6">
-        <v>0</v>
+        <v>357.46</v>
       </c>
       <c r="F5" s="7">
-        <v>31.87</v>
+        <v>538.94</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E6" s="6">
         <v>0</v>
       </c>
       <c r="F6" s="7">
-        <v>0</v>
+        <v>291.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6">
         <v>0</v>
       </c>
       <c r="F7" s="7">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="E8" s="6">
         <v>0</v>
@@ -1335,159 +1365,159 @@
     </row>
     <row r="9">
       <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="E9" s="6">
-        <v>0</v>
+        <v>134.61</v>
       </c>
       <c r="F9" s="7">
-        <v>0</v>
+        <v>168.42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
       </c>
       <c r="F10" s="7">
-        <v>714.71</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E11" s="6">
-        <v>0</v>
+        <v>20.5</v>
       </c>
       <c r="F11" s="7">
-        <v>1250</v>
+        <v>13.12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" s="6">
-        <v>0</v>
+        <v>64.43</v>
       </c>
       <c r="F12" s="7">
-        <v>631.2</v>
+        <v>8.97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" s="6">
-        <v>0</v>
+        <v>161.88</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>22.63</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="6" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E14" s="6">
-        <v>0</v>
+        <v>106.5</v>
       </c>
       <c r="F14" s="7">
-        <v>2340</v>
+        <v>13.42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E15" s="6">
-        <v>0</v>
+        <v>344.97</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>273.14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E16" s="6">
-        <v>0</v>
+        <v>892.89</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -1495,36 +1525,36 @@
     </row>
     <row r="17">
       <c r="A17" s="6" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E17" s="6">
-        <v>0</v>
+        <v>464.82</v>
       </c>
       <c r="F17" s="7">
-        <v>0</v>
+        <v>49.14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E18" s="6">
         <v>0</v>
@@ -1535,56 +1565,56 @@
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E19" s="6">
         <v>0</v>
       </c>
       <c r="F19" s="7">
-        <v>0</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>74</v>
-      </c>
       <c r="E20" s="6">
-        <v>0</v>
+        <v>19.97</v>
       </c>
       <c r="F20" s="7">
-        <v>1157</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E21" s="6">
         <v>0</v>
@@ -1595,33 +1625,33 @@
     </row>
     <row r="22">
       <c r="A22" s="6" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>77</v>
       </c>
       <c r="E22" s="6">
-        <v>0</v>
+        <v>106.5</v>
       </c>
       <c r="F22" s="7">
-        <v>0</v>
+        <v>13.42</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>79</v>
@@ -1630,44 +1660,44 @@
         <v>0</v>
       </c>
       <c r="F23" s="7">
-        <v>46</v>
+        <v>72.5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B24" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>81</v>
-      </c>
       <c r="E24" s="6">
-        <v>0</v>
+        <v>30.5</v>
       </c>
       <c r="F24" s="7">
-        <v>0</v>
+        <v>47.95</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="D25" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>83</v>
-      </c>
       <c r="E25" s="6">
-        <v>0</v>
+        <v>27.25</v>
       </c>
       <c r="F25" s="7">
         <v>0</v>
@@ -1675,201 +1705,301 @@
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E26" s="6">
-        <v>0</v>
+        <v>7320.96</v>
       </c>
       <c r="F26" s="7">
-        <v>0</v>
+        <v>351.67</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E27" s="6">
         <v>0</v>
       </c>
       <c r="F27" s="7">
-        <v>126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>27</v>
+        <v>53</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E28" s="6">
-        <v>0</v>
+        <v>387.58</v>
       </c>
       <c r="F28" s="7">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E29" s="6">
         <v>0</v>
       </c>
       <c r="F29" s="7">
-        <v>1562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>93</v>
-      </c>
       <c r="E30" s="6">
         <v>0</v>
       </c>
       <c r="F30" s="7">
-        <v>107</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="B31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>96</v>
-      </c>
       <c r="E31" s="6">
-        <v>0</v>
+        <v>47.26</v>
       </c>
       <c r="F31" s="7">
-        <v>0</v>
+        <v>98.25</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>98</v>
-      </c>
       <c r="E32" s="6">
-        <v>0</v>
+        <v>125.35</v>
       </c>
       <c r="F32" s="7">
-        <v>337</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D33" s="14" t="s">
         <v>99</v>
       </c>
       <c r="E33" s="6">
-        <v>0</v>
+        <v>211.42</v>
       </c>
       <c r="F33" s="7">
-        <v>66.5</v>
+        <v>1892.52</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="E34" s="6">
+        <v>0</v>
+      </c>
+      <c r="F34" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="6">
-        <v>0</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="15" t="s">
+      <c r="E35" s="6">
+        <v>115.31</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="16" t="s">
+      <c r="C36" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="15">
-        <v>0</v>
-      </c>
-      <c r="F35" s="17">
+      <c r="D36" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" s="6">
+        <v>32.92</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="6">
+        <v>107.89</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="15">
+        <v>900</v>
+      </c>
+      <c r="F40" s="17">
         <v>0</v>
       </c>
     </row>

</xml_diff>